<commit_message>
Corona Luft + Arbeitsstunden
</commit_message>
<xml_diff>
--- a/Arbeitsstunden.xlsx
+++ b/Arbeitsstunden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studium\E-Maker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C54178B-CE29-477A-9F86-B7C16B93ADDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD61B6FC-B9CA-490E-9581-4C5ECF560743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Startzeit</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Übung 108</t>
+  </si>
+  <si>
+    <t>Corona Lüftung Aufgaben</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497B6F7B-F5BE-2C40-940A-929DC888217C}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,6 +667,24 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44130</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D6" s="3">
+        <f>HOUR(C6)+MINUTE(C6)/60-HOUR(B6)-MINUTE(B6)/60+D5</f>
+        <v>10.666666666666666</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>